<commit_message>
make compatible with laravel-translation-loader (#17)
* wip

* fix tests

* edit exporter

* use in memory db

* wip

* wip

* wip

* wip

* wip

* wip

* wip

* Applied fixes from StyleCI
</commit_message>
<xml_diff>
--- a/tests/fixtures/fragments.xlsx
+++ b/tests/fixtures/fragments.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27309"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27106"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastiandedeyne/Sites/fragment-importer/tests/fixtures/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/freek/dev/github/blender-fragment-importer/tests/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12800" yWindow="460" windowWidth="25600" windowHeight="21060"/>
+    <workbookView xWindow="12800" yWindow="460" windowWidth="25600" windowHeight="21060" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="fragments" sheetId="1" r:id="rId1"/>
@@ -28,10 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
-  <si>
-    <t>name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
   <si>
     <t>contains_html</t>
   </si>
@@ -45,21 +42,6 @@
     <t>text_fr</t>
   </si>
   <si>
-    <t>fragment.withDescription</t>
-  </si>
-  <si>
-    <t>fragment.first</t>
-  </si>
-  <si>
-    <t>fragment.withHtml</t>
-  </si>
-  <si>
-    <t>fragment.second</t>
-  </si>
-  <si>
-    <t>fragment.emptyFields</t>
-  </si>
-  <si>
     <t>Lege velden</t>
   </si>
   <si>
@@ -87,13 +69,37 @@
     <t>Een</t>
   </si>
   <si>
-    <t>fragment.hidden</t>
-  </si>
-  <si>
     <t>Verborgen</t>
   </si>
   <si>
     <t>Caché</t>
+  </si>
+  <si>
+    <t>group</t>
+  </si>
+  <si>
+    <t>key</t>
+  </si>
+  <si>
+    <t>fragment</t>
+  </si>
+  <si>
+    <t>first</t>
+  </si>
+  <si>
+    <t>second</t>
+  </si>
+  <si>
+    <t>withHtml</t>
+  </si>
+  <si>
+    <t>withDescription</t>
+  </si>
+  <si>
+    <t>emptyFields</t>
+  </si>
+  <si>
+    <t>hidden</t>
   </si>
 </sst>
 </file>
@@ -140,12 +146,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -450,40 +457,42 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Z11"/>
+  <dimension ref="A1:AA11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="43.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="47.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="26" width="1.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="47.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="27" width="1.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -504,76 +513,92 @@
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA1" s="1"/>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
         <v>6</v>
       </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="E11" s="2"/>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="F11" s="2"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
@@ -587,40 +612,42 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Z2"/>
+  <dimension ref="A1:AA2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="53" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="80" customWidth="1"/>
-    <col min="5" max="5" width="133.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="26" width="1.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="80" customWidth="1"/>
+    <col min="6" max="6" width="133.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="27" width="1.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -641,25 +668,29 @@
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA1" s="1"/>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2">
         <v>0</v>
       </c>
-      <c r="D2" t="s">
-        <v>20</v>
-      </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <sortState ref="A2:E214">
-    <sortCondition ref="A2"/>
+  <sortState ref="B2:F214">
+    <sortCondition ref="B2"/>
   </sortState>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>